<commit_message>
POM Feb 4 th
</commit_message>
<xml_diff>
--- a/TestInput/Controller.xlsx
+++ b/TestInput/Controller.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="11616" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1152" windowWidth="11616" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -643,7 +643,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D4" s="20"/>
     </row>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>